<commit_message>
Deposit calculation refactoring next step
</commit_message>
<xml_diff>
--- a/Keeper/Utils/Deposits/DepositsCalculationScheme.xlsx
+++ b/Keeper/Utils/Deposits/DepositsCalculationScheme.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>показать отчет по депозиту</t>
   </si>
@@ -46,14 +46,65 @@
   </si>
   <si>
     <t>и общие суммы взносов, процентов, расходов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">нужна статистика и </t>
+  </si>
+  <si>
+    <t>нужен прогноз по месяцу и до конца</t>
+  </si>
+  <si>
+    <t>нужна статистика и</t>
+  </si>
+  <si>
+    <t>нужно определение какие %%</t>
+  </si>
+  <si>
+    <t>относятся к какому году</t>
+  </si>
+  <si>
+    <t>нужен прогноз по месяцу</t>
+  </si>
+  <si>
+    <t>статистика</t>
+  </si>
+  <si>
+    <t>отчеты</t>
+  </si>
+  <si>
+    <t>DepositReporter</t>
+  </si>
+  <si>
+    <t>DepositExcelReporter</t>
+  </si>
+  <si>
+    <t>составляет List&lt;String&gt; для отчета</t>
+  </si>
+  <si>
+    <t>составляет файл экселя</t>
+  </si>
+  <si>
+    <t>расчет</t>
+  </si>
+  <si>
+    <t>DepositCalculator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -82,8 +133,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -385,60 +437,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:I11"/>
+  <dimension ref="B3:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I6" t="s">
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="O6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="I7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
one more step in deposit procent calculation refactoring
</commit_message>
<xml_diff>
--- a/Keeper/Utils/Deposits/DepositsCalculationScheme.xlsx
+++ b/Keeper/Utils/Deposits/DepositsCalculationScheme.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>показать отчет по депозиту</t>
   </si>
@@ -51,9 +51,6 @@
     <t xml:space="preserve">нужна статистика и </t>
   </si>
   <si>
-    <t>нужен прогноз по месяцу и до конца</t>
-  </si>
-  <si>
     <t>нужна статистика и</t>
   </si>
   <si>
@@ -88,6 +85,33 @@
   </si>
   <si>
     <t>DepositCalculator</t>
+  </si>
+  <si>
+    <t>DepositCalculationAggregator</t>
+  </si>
+  <si>
+    <t>расчитывает проценты по вкладу</t>
+  </si>
+  <si>
+    <t>за каждый день</t>
+  </si>
+  <si>
+    <t xml:space="preserve">определяет какой период </t>
+  </si>
+  <si>
+    <t>уже оплачен, какой нет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">суммированием определяет </t>
+  </si>
+  <si>
+    <t>проценты за опред период</t>
+  </si>
+  <si>
+    <t>агрегирование</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> и до конца депозита</t>
   </si>
 </sst>
 </file>
@@ -437,99 +461,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O20"/>
+  <dimension ref="B3:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="28" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="22.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" t="s">
         <v>7</v>
       </c>
-      <c r="O5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="1" t="s">
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="P7" t="s">
         <v>9</v>
       </c>
-      <c r="O7" t="s">
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="O8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="O9" t="s">
+      <c r="K8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="K13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -544,12 +603,12 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
big improvements in deposit calculations
</commit_message>
<xml_diff>
--- a/Keeper/Utils/Deposits/DepositsCalculationScheme.xlsx
+++ b/Keeper/Utils/Deposits/DepositsCalculationScheme.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>показать отчет по депозиту</t>
   </si>
@@ -24,30 +24,15 @@
     <t>DepositViewModel</t>
   </si>
   <si>
-    <t>показать сводную форму по всем депозитам</t>
-  </si>
-  <si>
     <t>DepositsViewModel</t>
   </si>
   <si>
-    <t>показать ожидаемые доходы от депозитов</t>
-  </si>
-  <si>
     <t>MonthAnalysisViewModel</t>
   </si>
   <si>
     <t>DepositExtractor</t>
   </si>
   <si>
-    <t>Находит все операции по данному счету</t>
-  </si>
-  <si>
-    <t>и составляет таблицу ежедневных остатков</t>
-  </si>
-  <si>
-    <t>и общие суммы взносов, процентов, расходов</t>
-  </si>
-  <si>
     <t xml:space="preserve">нужна статистика и </t>
   </si>
   <si>
@@ -75,9 +60,6 @@
     <t>DepositExcelReporter</t>
   </si>
   <si>
-    <t>составляет List&lt;String&gt; для отчета</t>
-  </si>
-  <si>
     <t>составляет файл экселя</t>
   </si>
   <si>
@@ -90,9 +72,6 @@
     <t>DepositCalculationAggregator</t>
   </si>
   <si>
-    <t>расчитывает проценты по вкладу</t>
-  </si>
-  <si>
     <t>за каждый день</t>
   </si>
   <si>
@@ -112,6 +91,63 @@
   </si>
   <si>
     <t xml:space="preserve"> и до конца депозита</t>
+  </si>
+  <si>
+    <t>специализация</t>
+  </si>
+  <si>
+    <t>выбирает какой</t>
+  </si>
+  <si>
+    <t>калькулятор выбрать</t>
+  </si>
+  <si>
+    <t>для данного депозита</t>
+  </si>
+  <si>
+    <t>DepositApbStart</t>
+  </si>
+  <si>
+    <t>DepositVtbBonus</t>
+  </si>
+  <si>
+    <t>и т.д.</t>
+  </si>
+  <si>
+    <t>отдельные функции</t>
+  </si>
+  <si>
+    <t>CommonFunctionProvider</t>
+  </si>
+  <si>
+    <t>предоставляет функции</t>
+  </si>
+  <si>
+    <t>одинаковые для разных</t>
+  </si>
+  <si>
+    <t>вкладов</t>
+  </si>
+  <si>
+    <t>показать сводную форму</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> по всем депозитам</t>
+  </si>
+  <si>
+    <t xml:space="preserve">показать ожидаемые </t>
+  </si>
+  <si>
+    <t>доходы от депозитов</t>
+  </si>
+  <si>
+    <t>составляет List&lt;String&gt;</t>
+  </si>
+  <si>
+    <t>расчитывает %% по вкладу</t>
+  </si>
+  <si>
+    <t>Находит все операции по данному счету и составляет таблицу ежедневных остатков и общие суммы взносов, процентов, расходов</t>
   </si>
 </sst>
 </file>
@@ -157,9 +193,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -461,159 +500,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:P20"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="28" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="P3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P5" t="s">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="H14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
         <v>18</v>
       </c>
-      <c r="P7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" t="s">
-        <v>30</v>
-      </c>
-      <c r="M8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="K9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>14</v>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <mergeCells count="1">
+    <mergeCell ref="J5:J12"/>
+  </mergeCells>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="84" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
improved month analysis for deposits in future periods
</commit_message>
<xml_diff>
--- a/Keeper/Utils/Deposits/DepositsCalculationScheme.xlsx
+++ b/Keeper/Utils/Deposits/DepositsCalculationScheme.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>показать отчет по депозиту</t>
   </si>
@@ -72,9 +72,6 @@
     <t>DepositCalculationAggregator</t>
   </si>
   <si>
-    <t>за каждый день</t>
-  </si>
-  <si>
     <t xml:space="preserve">определяет какой период </t>
   </si>
   <si>
@@ -93,42 +90,9 @@
     <t xml:space="preserve"> и до конца депозита</t>
   </si>
   <si>
-    <t>специализация</t>
-  </si>
-  <si>
-    <t>выбирает какой</t>
-  </si>
-  <si>
-    <t>калькулятор выбрать</t>
-  </si>
-  <si>
-    <t>для данного депозита</t>
-  </si>
-  <si>
-    <t>DepositApbStart</t>
-  </si>
-  <si>
-    <t>DepositVtbBonus</t>
-  </si>
-  <si>
-    <t>и т.д.</t>
-  </si>
-  <si>
     <t>отдельные функции</t>
   </si>
   <si>
-    <t>CommonFunctionProvider</t>
-  </si>
-  <si>
-    <t>предоставляет функции</t>
-  </si>
-  <si>
-    <t>одинаковые для разных</t>
-  </si>
-  <si>
-    <t>вкладов</t>
-  </si>
-  <si>
     <t>показать сводную форму</t>
   </si>
   <si>
@@ -144,10 +108,67 @@
     <t>составляет List&lt;String&gt;</t>
   </si>
   <si>
-    <t>расчитывает %% по вкладу</t>
-  </si>
-  <si>
     <t>Находит все операции по данному счету и составляет таблицу ежедневных остатков и общие суммы взносов, процентов, расходов</t>
+  </si>
+  <si>
+    <t>DepositCalculationFunctions</t>
+  </si>
+  <si>
+    <t>вспомогательные функции</t>
+  </si>
+  <si>
+    <t>для расчета процентов</t>
+  </si>
+  <si>
+    <t>считает ежедневные проценты, добавляя будущие операции капитализации/выплаты процентов, не изменяя при этом поля содержащие суммы фактически выплаченных процентов</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     BankDepositOffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          BankDepositCalculatingRules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          ObservableCollection&lt;DepositRateLine&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     DepositCalculationData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          DepositStates State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          List&lt;DepositTransaction&gt; Traffic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          List&lt;DepositDailyLine&gt; DailyTable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal TotalMyIns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal TotalPercent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal TotalMyOuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal CurrentBalance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal CurrentProfit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal EstimatedProcentsInThisMonth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal EstimatedProcents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          decimal EstimatedProfitInUsd</t>
   </si>
 </sst>
 </file>
@@ -503,10 +524,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:J30"/>
+  <dimension ref="B2:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,216 +535,267 @@
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="1" t="s">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="H14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="H15" t="s">
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H26" t="s">
+      <c r="F31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="1" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H30" t="s">
-        <v>36</v>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="J5:J12"/>
+  <mergeCells count="2">
+    <mergeCell ref="G5:G12"/>
+    <mergeCell ref="F19:F27"/>
   </mergeCells>
   <printOptions gridLines="1"/>
-  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="84" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="96" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>